<commit_message>
Create Feature training new Model contain HTML and update app.py
</commit_message>
<xml_diff>
--- a/Web_Application/Dataset/CompanyCV.xlsx
+++ b/Web_Application/Dataset/CompanyCV.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451F77F2-028F-4D85-BF3B-2AB77F228234}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB1CD5F-7299-436D-9DE7-A005FA2A0D17}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -578,11 +578,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -866,7 +871,7 @@
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:N5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,42 +881,45 @@
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1"/>
@@ -944,7 +952,7 @@
       <c r="I2">
         <v>2</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>3.7431898121336489</v>
       </c>
       <c r="K2" t="s">
@@ -979,7 +987,7 @@
       <c r="I3">
         <v>4</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="2">
         <v>2.6079465663449821</v>
       </c>
       <c r="K3" t="s">
@@ -1014,7 +1022,7 @@
       <c r="I4">
         <v>6</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>2.62499288327193</v>
       </c>
       <c r="K4" t="s">
@@ -1049,7 +1057,7 @@
       <c r="I5">
         <v>0</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>2.6866176850376373</v>
       </c>
       <c r="K5" t="s">
@@ -1084,7 +1092,7 @@
       <c r="I6">
         <v>5</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <v>2.7759177900997161</v>
       </c>
       <c r="K6" t="s">
@@ -1119,7 +1127,7 @@
       <c r="I7">
         <v>3</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <v>3.6193495348036286</v>
       </c>
       <c r="K7" t="s">
@@ -1154,7 +1162,7 @@
       <c r="I8">
         <v>0</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <v>2.9158088140391176</v>
       </c>
       <c r="K8" t="s">
@@ -1189,7 +1197,7 @@
       <c r="I9">
         <v>6</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <v>3.9086024167443965</v>
       </c>
       <c r="K9" t="s">
@@ -1224,7 +1232,7 @@
       <c r="I10">
         <v>2</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <v>3.426792859527247</v>
       </c>
       <c r="K10" t="s">
@@ -1259,7 +1267,7 @@
       <c r="I11">
         <v>6</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <v>3.2064952241030573</v>
       </c>
       <c r="K11" t="s">
@@ -1294,7 +1302,7 @@
       <c r="I12">
         <v>4</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="2">
         <v>3.2413715211250729</v>
       </c>
       <c r="K12" t="s">
@@ -1329,7 +1337,7 @@
       <c r="I13">
         <v>4</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="2">
         <v>2.9622297333219301</v>
       </c>
       <c r="K13" t="s">
@@ -1364,7 +1372,7 @@
       <c r="I14">
         <v>3</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="2">
         <v>3.8906670915577837</v>
       </c>
       <c r="K14" t="s">
@@ -1399,7 +1407,7 @@
       <c r="I15">
         <v>0</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="2">
         <v>3.7165239781875177</v>
       </c>
       <c r="K15" t="s">
@@ -1434,7 +1442,7 @@
       <c r="I16">
         <v>0</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="2">
         <v>2.9686834535567241</v>
       </c>
       <c r="K16" t="s">
@@ -1469,7 +1477,7 @@
       <c r="I17">
         <v>4</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="2">
         <v>3.7244906100768338</v>
       </c>
       <c r="K17" t="s">
@@ -1504,7 +1512,7 @@
       <c r="I18">
         <v>2</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="2">
         <v>3.8098128024196178</v>
       </c>
       <c r="K18" t="s">
@@ -1539,7 +1547,7 @@
       <c r="I19">
         <v>3</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="2">
         <v>2.564146253414064</v>
       </c>
       <c r="K19" t="s">
@@ -1574,7 +1582,7 @@
       <c r="I20">
         <v>5</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="2">
         <v>2.6495945270788921</v>
       </c>
       <c r="K20" t="s">
@@ -1609,7 +1617,7 @@
       <c r="I21">
         <v>4</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="2">
         <v>3.9989414569853605</v>
       </c>
       <c r="K21" t="s">
@@ -1644,7 +1652,7 @@
       <c r="I22">
         <v>0</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="2">
         <v>3.8873062252724129</v>
       </c>
       <c r="K22" t="s">
@@ -1679,7 +1687,7 @@
       <c r="I23">
         <v>3</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="2">
         <v>3.7607847031721824</v>
       </c>
       <c r="K23" t="s">
@@ -1714,7 +1722,7 @@
       <c r="I24">
         <v>3</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="2">
         <v>3.8809191245528822</v>
       </c>
       <c r="K24" t="s">
@@ -1749,7 +1757,7 @@
       <c r="I25">
         <v>5</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="2">
         <v>3.8741740632140003</v>
       </c>
       <c r="K25" t="s">
@@ -1784,7 +1792,7 @@
       <c r="I26">
         <v>3</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="2">
         <v>2.5438025639197597</v>
       </c>
       <c r="K26" t="s">
@@ -1819,7 +1827,7 @@
       <c r="I27">
         <v>5</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="2">
         <v>2.9290556448042735</v>
       </c>
       <c r="K27" t="s">
@@ -1854,7 +1862,7 @@
       <c r="I28">
         <v>5</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="2">
         <v>2.60812681737977</v>
       </c>
       <c r="K28" t="s">
@@ -1889,7 +1897,7 @@
       <c r="I29">
         <v>3</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="2">
         <v>3.6682808179351851</v>
       </c>
       <c r="K29" t="s">
@@ -1924,7 +1932,7 @@
       <c r="I30">
         <v>4</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="2">
         <v>3.2009440287086854</v>
       </c>
       <c r="K30" t="s">
@@ -1959,7 +1967,7 @@
       <c r="I31">
         <v>3</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="2">
         <v>3.9916355018785135</v>
       </c>
       <c r="K31" t="s">
@@ -1994,7 +2002,7 @@
       <c r="I32">
         <v>3</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="2">
         <v>3.7324292025987345</v>
       </c>
       <c r="K32" t="s">
@@ -2029,7 +2037,7 @@
       <c r="I33">
         <v>6</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="2">
         <v>2.8421992218044996</v>
       </c>
       <c r="K33" t="s">
@@ -2064,7 +2072,7 @@
       <c r="I34">
         <v>4</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="2">
         <v>2.7793749549745237</v>
       </c>
       <c r="K34" t="s">
@@ -2099,7 +2107,7 @@
       <c r="I35">
         <v>6</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="2">
         <v>3.4931382163894744</v>
       </c>
       <c r="K35" t="s">
@@ -2134,7 +2142,7 @@
       <c r="I36">
         <v>5</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36" s="2">
         <v>2.5930726626240435</v>
       </c>
       <c r="K36" t="s">
@@ -2169,7 +2177,7 @@
       <c r="I37">
         <v>2</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J37" s="2">
         <v>2.9545328761992176</v>
       </c>
       <c r="K37" t="s">
@@ -2204,7 +2212,7 @@
       <c r="I38">
         <v>2</v>
       </c>
-      <c r="J38" s="3">
+      <c r="J38" s="2">
         <v>2.841262594975078</v>
       </c>
       <c r="K38" t="s">
@@ -2239,7 +2247,7 @@
       <c r="I39">
         <v>0</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39" s="2">
         <v>3.8188426719982473</v>
       </c>
       <c r="K39" t="s">
@@ -2274,7 +2282,7 @@
       <c r="I40">
         <v>6</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="2">
         <v>3.14610919448209</v>
       </c>
       <c r="K40" t="s">
@@ -2309,7 +2317,7 @@
       <c r="I41">
         <v>4</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J41" s="2">
         <v>2.6554554713004288</v>
       </c>
       <c r="K41" t="s">
@@ -2344,7 +2352,7 @@
       <c r="I42">
         <v>0</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="2">
         <v>3.8324393169077018</v>
       </c>
       <c r="K42" t="s">
@@ -2379,7 +2387,7 @@
       <c r="I43">
         <v>5</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J43" s="2">
         <v>3.0966970151721496</v>
       </c>
       <c r="K43" t="s">
@@ -2414,7 +2422,7 @@
       <c r="I44">
         <v>3</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44" s="2">
         <v>3.7629745836030355</v>
       </c>
       <c r="K44" t="s">
@@ -2449,7 +2457,7 @@
       <c r="I45">
         <v>6</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J45" s="2">
         <v>3.8794399709742908</v>
       </c>
       <c r="K45" t="s">
@@ -2484,7 +2492,7 @@
       <c r="I46">
         <v>3</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J46" s="2">
         <v>2.6168591612010061</v>
       </c>
       <c r="K46" t="s">
@@ -2519,7 +2527,7 @@
       <c r="I47">
         <v>4</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47" s="2">
         <v>3.3750062940520618</v>
       </c>
       <c r="K47" t="s">
@@ -2554,7 +2562,7 @@
       <c r="I48">
         <v>3</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48" s="2">
         <v>3.3292091977841789</v>
       </c>
       <c r="K48" t="s">
@@ -2589,7 +2597,7 @@
       <c r="I49">
         <v>4</v>
       </c>
-      <c r="J49" s="3">
+      <c r="J49" s="2">
         <v>3.4454660342670125</v>
       </c>
       <c r="K49" t="s">
@@ -2624,7 +2632,7 @@
       <c r="I50">
         <v>6</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J50" s="2">
         <v>3.994225584758321</v>
       </c>
       <c r="K50" t="s">
@@ -2659,7 +2667,7 @@
       <c r="I51">
         <v>0</v>
       </c>
-      <c r="J51" s="3">
+      <c r="J51" s="2">
         <v>2.7598149705632182</v>
       </c>
       <c r="K51" t="s">
@@ -2694,7 +2702,7 @@
       <c r="I52">
         <v>0</v>
       </c>
-      <c r="J52" s="3">
+      <c r="J52" s="2">
         <v>2.559291675616866</v>
       </c>
       <c r="K52" t="s">
@@ -2729,7 +2737,7 @@
       <c r="I53">
         <v>6</v>
       </c>
-      <c r="J53" s="3">
+      <c r="J53" s="2">
         <v>3.9575892807584054</v>
       </c>
       <c r="K53" t="s">
@@ -2764,7 +2772,7 @@
       <c r="I54">
         <v>2</v>
       </c>
-      <c r="J54" s="3">
+      <c r="J54" s="2">
         <v>3.1491816321549662</v>
       </c>
       <c r="K54" t="s">
@@ -2799,7 +2807,7 @@
       <c r="I55">
         <v>4</v>
       </c>
-      <c r="J55" s="3">
+      <c r="J55" s="2">
         <v>2.6530912908197268</v>
       </c>
       <c r="K55" t="s">
@@ -2834,7 +2842,7 @@
       <c r="I56">
         <v>3</v>
       </c>
-      <c r="J56" s="3">
+      <c r="J56" s="2">
         <v>3.3559148019089884</v>
       </c>
       <c r="K56" t="s">
@@ -2869,7 +2877,7 @@
       <c r="I57">
         <v>0</v>
       </c>
-      <c r="J57" s="3">
+      <c r="J57" s="2">
         <v>3.0016861426787553</v>
       </c>
       <c r="K57" t="s">
@@ -2904,7 +2912,7 @@
       <c r="I58">
         <v>4</v>
       </c>
-      <c r="J58" s="3">
+      <c r="J58" s="2">
         <v>2.5325032323748422</v>
       </c>
       <c r="K58" t="s">
@@ -2939,7 +2947,7 @@
       <c r="I59">
         <v>3</v>
       </c>
-      <c r="J59" s="3">
+      <c r="J59" s="2">
         <v>3.3712860712019612</v>
       </c>
       <c r="K59" t="s">
@@ -2974,7 +2982,7 @@
       <c r="I60">
         <v>5</v>
       </c>
-      <c r="J60" s="3">
+      <c r="J60" s="2">
         <v>3.3449528233112478</v>
       </c>
       <c r="K60" t="s">
@@ -3009,7 +3017,7 @@
       <c r="I61">
         <v>6</v>
       </c>
-      <c r="J61" s="3">
+      <c r="J61" s="2">
         <v>3.3611089573688222</v>
       </c>
       <c r="K61" t="s">
@@ -3044,7 +3052,7 @@
       <c r="I62">
         <v>0</v>
       </c>
-      <c r="J62" s="3">
+      <c r="J62" s="2">
         <v>3.6189806034337879</v>
       </c>
       <c r="K62" t="s">
@@ -3079,7 +3087,7 @@
       <c r="I63">
         <v>2</v>
       </c>
-      <c r="J63" s="3">
+      <c r="J63" s="2">
         <v>3.9878855301220124</v>
       </c>
       <c r="K63" t="s">
@@ -3114,7 +3122,7 @@
       <c r="I64">
         <v>0</v>
       </c>
-      <c r="J64" s="3">
+      <c r="J64" s="2">
         <v>2.5065395508284825</v>
       </c>
       <c r="K64" t="s">
@@ -3149,7 +3157,7 @@
       <c r="I65">
         <v>0</v>
       </c>
-      <c r="J65" s="3">
+      <c r="J65" s="2">
         <v>2.9725223810546328</v>
       </c>
       <c r="K65" t="s">
@@ -3184,7 +3192,7 @@
       <c r="I66">
         <v>0</v>
       </c>
-      <c r="J66" s="3">
+      <c r="J66" s="2">
         <v>3.4351476714470932</v>
       </c>
       <c r="K66" t="s">
@@ -3219,7 +3227,7 @@
       <c r="I67">
         <v>4</v>
       </c>
-      <c r="J67" s="3">
+      <c r="J67" s="2">
         <v>3.5070172624788185</v>
       </c>
       <c r="K67" t="s">
@@ -3254,7 +3262,7 @@
       <c r="I68">
         <v>3</v>
       </c>
-      <c r="J68" s="3">
+      <c r="J68" s="2">
         <v>3.2434803817867621</v>
       </c>
       <c r="K68" t="s">
@@ -3289,7 +3297,7 @@
       <c r="I69">
         <v>3</v>
       </c>
-      <c r="J69" s="3">
+      <c r="J69" s="2">
         <v>3.6709352619360445</v>
       </c>
       <c r="K69" t="s">
@@ -3324,7 +3332,7 @@
       <c r="I70">
         <v>6</v>
       </c>
-      <c r="J70" s="3">
+      <c r="J70" s="2">
         <v>3.6167920383629206</v>
       </c>
       <c r="K70" t="s">
@@ -3359,7 +3367,7 @@
       <c r="I71">
         <v>6</v>
       </c>
-      <c r="J71" s="3">
+      <c r="J71" s="2">
         <v>3.7963312595042886</v>
       </c>
       <c r="K71" t="s">
@@ -3394,7 +3402,7 @@
       <c r="I72">
         <v>2</v>
       </c>
-      <c r="J72" s="3">
+      <c r="J72" s="2">
         <v>3.7960445010354142</v>
       </c>
       <c r="K72" t="s">
@@ -3429,7 +3437,7 @@
       <c r="I73">
         <v>6</v>
       </c>
-      <c r="J73" s="3">
+      <c r="J73" s="2">
         <v>2.8180815116283169</v>
       </c>
       <c r="K73" t="s">
@@ -3464,7 +3472,7 @@
       <c r="I74">
         <v>5</v>
       </c>
-      <c r="J74" s="3">
+      <c r="J74" s="2">
         <v>2.5667351077986114</v>
       </c>
       <c r="K74" t="s">
@@ -3499,7 +3507,7 @@
       <c r="I75">
         <v>4</v>
       </c>
-      <c r="J75" s="3">
+      <c r="J75" s="2">
         <v>3.7870187551761871</v>
       </c>
       <c r="K75" t="s">
@@ -3534,7 +3542,7 @@
       <c r="I76">
         <v>3</v>
       </c>
-      <c r="J76" s="3">
+      <c r="J76" s="2">
         <v>3.1740226750568468</v>
       </c>
       <c r="K76" t="s">
@@ -3569,7 +3577,7 @@
       <c r="I77">
         <v>0</v>
       </c>
-      <c r="J77" s="3">
+      <c r="J77" s="2">
         <v>3.3522522876930592</v>
       </c>
       <c r="K77" t="s">
@@ -3604,7 +3612,7 @@
       <c r="I78">
         <v>0</v>
       </c>
-      <c r="J78" s="3">
+      <c r="J78" s="2">
         <v>3.2601392591675151</v>
       </c>
       <c r="K78" t="s">
@@ -3639,7 +3647,7 @@
       <c r="I79">
         <v>6</v>
       </c>
-      <c r="J79" s="3">
+      <c r="J79" s="2">
         <v>3.2961516950490415</v>
       </c>
       <c r="K79" t="s">
@@ -3674,7 +3682,7 @@
       <c r="I80">
         <v>0</v>
       </c>
-      <c r="J80" s="3">
+      <c r="J80" s="2">
         <v>3.1369798551674104</v>
       </c>
       <c r="K80" t="s">
@@ -3709,7 +3717,7 @@
       <c r="I81">
         <v>5</v>
       </c>
-      <c r="J81" s="3">
+      <c r="J81" s="2">
         <v>3.0630341366240956</v>
       </c>
       <c r="K81" t="s">
@@ -3744,7 +3752,7 @@
       <c r="I82">
         <v>3</v>
       </c>
-      <c r="J82" s="3">
+      <c r="J82" s="2">
         <v>3.1941124128302372</v>
       </c>
       <c r="K82" t="s">
@@ -3779,7 +3787,7 @@
       <c r="I83">
         <v>5</v>
       </c>
-      <c r="J83" s="3">
+      <c r="J83" s="2">
         <v>2.5904722891214176</v>
       </c>
       <c r="K83" t="s">
@@ -3814,7 +3822,7 @@
       <c r="I84">
         <v>5</v>
       </c>
-      <c r="J84" s="3">
+      <c r="J84" s="2">
         <v>3.0450701915706508</v>
       </c>
       <c r="K84" t="s">
@@ -3849,7 +3857,7 @@
       <c r="I85">
         <v>3</v>
       </c>
-      <c r="J85" s="3">
+      <c r="J85" s="2">
         <v>3.4075109227317713</v>
       </c>
       <c r="K85" t="s">
@@ -3884,7 +3892,7 @@
       <c r="I86">
         <v>4</v>
       </c>
-      <c r="J86" s="3">
+      <c r="J86" s="2">
         <v>2.8559351695581081</v>
       </c>
       <c r="K86" t="s">
@@ -3919,7 +3927,7 @@
       <c r="I87">
         <v>0</v>
       </c>
-      <c r="J87" s="3">
+      <c r="J87" s="2">
         <v>3.1983355003283132</v>
       </c>
       <c r="K87" t="s">
@@ -3954,7 +3962,7 @@
       <c r="I88">
         <v>0</v>
       </c>
-      <c r="J88" s="3">
+      <c r="J88" s="2">
         <v>3.2683751829785996</v>
       </c>
       <c r="K88" t="s">
@@ -3989,7 +3997,7 @@
       <c r="I89">
         <v>2</v>
       </c>
-      <c r="J89" s="3">
+      <c r="J89" s="2">
         <v>2.6655637535945558</v>
       </c>
       <c r="K89" t="s">
@@ -4024,7 +4032,7 @@
       <c r="I90">
         <v>3</v>
       </c>
-      <c r="J90" s="3">
+      <c r="J90" s="2">
         <v>2.5105472309464041</v>
       </c>
       <c r="K90" t="s">
@@ -4059,7 +4067,7 @@
       <c r="I91">
         <v>2</v>
       </c>
-      <c r="J91" s="3">
+      <c r="J91" s="2">
         <v>3.4251721111003839</v>
       </c>
       <c r="K91" t="s">
@@ -4094,7 +4102,7 @@
       <c r="I92">
         <v>6</v>
       </c>
-      <c r="J92" s="3">
+      <c r="J92" s="2">
         <v>2.9275156560655446</v>
       </c>
       <c r="K92" t="s">
@@ -4129,7 +4137,7 @@
       <c r="I93">
         <v>6</v>
       </c>
-      <c r="J93" s="3">
+      <c r="J93" s="2">
         <v>3.3180790525465498</v>
       </c>
       <c r="K93" t="s">
@@ -4164,7 +4172,7 @@
       <c r="I94">
         <v>3</v>
       </c>
-      <c r="J94" s="3">
+      <c r="J94" s="2">
         <v>3.2074649983876187</v>
       </c>
       <c r="K94" t="s">
@@ -4199,7 +4207,7 @@
       <c r="I95">
         <v>4</v>
       </c>
-      <c r="J95" s="3">
+      <c r="J95" s="2">
         <v>3.8022402580308592</v>
       </c>
       <c r="K95" t="s">
@@ -4234,7 +4242,7 @@
       <c r="I96">
         <v>6</v>
       </c>
-      <c r="J96" s="3">
+      <c r="J96" s="2">
         <v>3.7052192397407753</v>
       </c>
       <c r="K96" t="s">
@@ -4269,7 +4277,7 @@
       <c r="I97">
         <v>2</v>
       </c>
-      <c r="J97" s="3">
+      <c r="J97" s="2">
         <v>3.3631245571439399</v>
       </c>
       <c r="K97" t="s">
@@ -4304,7 +4312,7 @@
       <c r="I98">
         <v>0</v>
       </c>
-      <c r="J98" s="3">
+      <c r="J98" s="2">
         <v>2.8019900545672547</v>
       </c>
       <c r="K98" t="s">
@@ -4339,7 +4347,7 @@
       <c r="I99">
         <v>4</v>
       </c>
-      <c r="J99" s="3">
+      <c r="J99" s="2">
         <v>3.4292402024119735</v>
       </c>
       <c r="K99" t="s">
@@ -4374,7 +4382,7 @@
       <c r="I100">
         <v>2</v>
       </c>
-      <c r="J100" s="3">
+      <c r="J100" s="2">
         <v>3.7246779254350808</v>
       </c>
       <c r="K100" t="s">

</xml_diff>